<commit_message>
antes calcular receita e despesas
</commit_message>
<xml_diff>
--- a/Arquivos/Acerto AP.xlsx
+++ b/Arquivos/Acerto AP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\Xampp\htdocs\Testes\Controle_Financeiro\Arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6F190A-8F9C-4EEF-B27D-112C670E3DDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942BB9E4-69C7-45FB-ABDC-084D22D6AA18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{259B233A-82EC-4420-B52E-363BB860C0EF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="12360" xr2:uid="{259B233A-82EC-4420-B52E-363BB860C0EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="26">
   <si>
     <t>Descricao</t>
   </si>
@@ -117,7 +117,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
@@ -205,7 +206,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -222,6 +223,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -666,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A21A576-F462-4417-98D5-276940579365}">
   <dimension ref="B2:H62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="L60" sqref="L60"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1463,7 +1465,9 @@
       </c>
     </row>
     <row r="37" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="9"/>
+      <c r="B37" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="C37" s="8">
         <v>43891</v>
       </c>
@@ -1474,7 +1478,7 @@
         <v>17</v>
       </c>
       <c r="F37" s="7">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="G37" s="7"/>
       <c r="H37" s="7">
@@ -1482,7 +1486,9 @@
       </c>
     </row>
     <row r="38" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="9"/>
+      <c r="B38" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="C38" s="8">
         <v>43900</v>
       </c>
@@ -1493,17 +1499,20 @@
         <v>16</v>
       </c>
       <c r="F38" s="7">
-        <v>1519.48</v>
-      </c>
-      <c r="G38" s="7">
-        <v>909.5</v>
+        <v>1342.33</v>
+      </c>
+      <c r="G38" s="12">
+        <f>(SUM(F37:F38)-SUM(H37:H38))</f>
+        <v>1142.33</v>
       </c>
       <c r="H38" s="7">
-        <v>600</v>
+        <v>700</v>
       </c>
     </row>
     <row r="39" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="9"/>
+      <c r="B39" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="C39" s="8">
         <v>43556</v>
       </c>
@@ -1514,7 +1523,7 @@
         <v>17</v>
       </c>
       <c r="F39" s="7">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="G39" s="7"/>
       <c r="H39" s="7">
@@ -1522,7 +1531,9 @@
       </c>
     </row>
     <row r="40" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="9"/>
+      <c r="B40" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="C40" s="8">
         <v>43931</v>
       </c>
@@ -1533,17 +1544,20 @@
         <v>16</v>
       </c>
       <c r="F40" s="7">
-        <v>1519.48</v>
-      </c>
-      <c r="G40" s="7">
-        <v>909.5</v>
+        <v>1347.64</v>
+      </c>
+      <c r="G40" s="12">
+        <f>(SUM(F39:F40)-SUM(H39:H40))</f>
+        <v>1347.6400000000003</v>
       </c>
       <c r="H40" s="7">
-        <v>600</v>
+        <v>700</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="9"/>
+      <c r="B41" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="C41" s="8">
         <v>43952</v>
       </c>
@@ -1554,7 +1568,7 @@
         <v>17</v>
       </c>
       <c r="F41" s="7">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="G41" s="7"/>
       <c r="H41" s="7">
@@ -1562,7 +1576,9 @@
       </c>
     </row>
     <row r="42" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="9"/>
+      <c r="B42" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="C42" s="8">
         <v>43961</v>
       </c>
@@ -1573,17 +1589,20 @@
         <v>16</v>
       </c>
       <c r="F42" s="7">
-        <v>1519.48</v>
-      </c>
-      <c r="G42" s="7">
-        <v>909.5</v>
+        <v>1350.27</v>
+      </c>
+      <c r="G42" s="12">
+        <f t="shared" ref="G42" si="0">(SUM(F41:F42)-SUM(H41:H42))</f>
+        <v>1350.27</v>
       </c>
       <c r="H42" s="7">
-        <v>600</v>
+        <v>700</v>
       </c>
     </row>
     <row r="43" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="9"/>
+      <c r="B43" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="C43" s="8">
         <v>43983</v>
       </c>
@@ -1594,7 +1613,7 @@
         <v>17</v>
       </c>
       <c r="F43" s="7">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="G43" s="7"/>
       <c r="H43" s="7">
@@ -1602,7 +1621,9 @@
       </c>
     </row>
     <row r="44" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="9"/>
+      <c r="B44" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="C44" s="8">
         <v>43992</v>
       </c>
@@ -1613,17 +1634,20 @@
         <v>16</v>
       </c>
       <c r="F44" s="7">
-        <v>1519.48</v>
-      </c>
-      <c r="G44" s="7">
-        <v>909.5</v>
+        <v>1354.1</v>
+      </c>
+      <c r="G44" s="12">
+        <f t="shared" ref="G44" si="1">(SUM(F43:F44)-SUM(H43:H44))</f>
+        <v>1554.1</v>
       </c>
       <c r="H44" s="7">
-        <v>600</v>
+        <v>700</v>
       </c>
     </row>
     <row r="45" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="9"/>
+      <c r="B45" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="C45" s="8">
         <v>44013</v>
       </c>
@@ -1634,7 +1658,7 @@
         <v>17</v>
       </c>
       <c r="F45" s="7">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="G45" s="7"/>
       <c r="H45" s="7">
@@ -1642,7 +1666,9 @@
       </c>
     </row>
     <row r="46" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="9"/>
+      <c r="B46" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="C46" s="8">
         <v>44022</v>
       </c>
@@ -1653,17 +1679,20 @@
         <v>16</v>
       </c>
       <c r="F46" s="7">
-        <v>1519.48</v>
-      </c>
-      <c r="G46" s="7">
-        <v>909.5</v>
+        <v>1356.83</v>
+      </c>
+      <c r="G46" s="12">
+        <f t="shared" ref="G46" si="2">(SUM(F45:F46)-SUM(H45:H46))</f>
+        <v>1556.83</v>
       </c>
       <c r="H46" s="7">
-        <v>600</v>
+        <v>700</v>
       </c>
     </row>
     <row r="47" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="9"/>
+      <c r="B47" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="C47" s="8">
         <v>44044</v>
       </c>
@@ -1674,7 +1703,7 @@
         <v>17</v>
       </c>
       <c r="F47" s="7">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="G47" s="7"/>
       <c r="H47" s="7">
@@ -1682,7 +1711,9 @@
       </c>
     </row>
     <row r="48" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="9"/>
+      <c r="B48" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="C48" s="8">
         <v>44053</v>
       </c>
@@ -1693,17 +1724,20 @@
         <v>16</v>
       </c>
       <c r="F48" s="7">
-        <v>1519.48</v>
-      </c>
-      <c r="G48" s="7">
-        <v>909.5</v>
+        <v>1305.82</v>
+      </c>
+      <c r="G48" s="12">
+        <f t="shared" ref="G48" si="3">(SUM(F47:F48)-SUM(H47:H48))</f>
+        <v>1505.8199999999997</v>
       </c>
       <c r="H48" s="7">
-        <v>600</v>
+        <v>700</v>
       </c>
     </row>
     <row r="49" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="9"/>
+      <c r="B49" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="C49" s="8">
         <v>44075</v>
       </c>
@@ -1714,7 +1748,7 @@
         <v>17</v>
       </c>
       <c r="F49" s="7">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="G49" s="7"/>
       <c r="H49" s="7">
@@ -1722,7 +1756,9 @@
       </c>
     </row>
     <row r="50" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="9"/>
+      <c r="B50" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="C50" s="8">
         <v>44084</v>
       </c>
@@ -1733,13 +1769,14 @@
         <v>16</v>
       </c>
       <c r="F50" s="7">
-        <v>1519.48</v>
-      </c>
-      <c r="G50" s="7">
-        <v>909.5</v>
+        <v>1321.53</v>
+      </c>
+      <c r="G50" s="12">
+        <f t="shared" ref="G50" si="4">(SUM(F49:F50)-SUM(H49:H50))</f>
+        <v>1521.5299999999997</v>
       </c>
       <c r="H50" s="7">
-        <v>600</v>
+        <v>700</v>
       </c>
     </row>
     <row r="51" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1754,7 +1791,7 @@
         <v>17</v>
       </c>
       <c r="F51" s="7">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="G51" s="7"/>
       <c r="H51" s="7">
@@ -1773,13 +1810,14 @@
         <v>16</v>
       </c>
       <c r="F52" s="7">
-        <v>1519.48</v>
-      </c>
-      <c r="G52" s="7">
-        <v>909.5</v>
+        <v>1321.53</v>
+      </c>
+      <c r="G52" s="12">
+        <f t="shared" ref="G52" si="5">(SUM(F51:F52)-SUM(H51:H52))</f>
+        <v>1521.5299999999997</v>
       </c>
       <c r="H52" s="7">
-        <v>600</v>
+        <v>700</v>
       </c>
     </row>
     <row r="53" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1794,7 +1832,7 @@
         <v>17</v>
       </c>
       <c r="F53" s="7">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="G53" s="7"/>
       <c r="H53" s="7">
@@ -1813,13 +1851,14 @@
         <v>16</v>
       </c>
       <c r="F54" s="7">
-        <v>1519.48</v>
-      </c>
-      <c r="G54" s="7">
-        <v>909.5</v>
+        <v>1321.53</v>
+      </c>
+      <c r="G54" s="12">
+        <f t="shared" ref="G54" si="6">(SUM(F53:F54)-SUM(H53:H54))</f>
+        <v>1521.5299999999997</v>
       </c>
       <c r="H54" s="7">
-        <v>600</v>
+        <v>700</v>
       </c>
     </row>
     <row r="55" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1834,7 +1873,7 @@
         <v>17</v>
       </c>
       <c r="F55" s="7">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="G55" s="7"/>
       <c r="H55" s="7">
@@ -1853,13 +1892,14 @@
         <v>16</v>
       </c>
       <c r="F56" s="7">
-        <v>1519.48</v>
-      </c>
-      <c r="G56" s="7">
-        <v>909.5</v>
+        <v>1321.53</v>
+      </c>
+      <c r="G56" s="12">
+        <f t="shared" ref="G56" si="7">(SUM(F55:F56)-SUM(H55:H56))</f>
+        <v>1521.5299999999997</v>
       </c>
       <c r="H56" s="7">
-        <v>600</v>
+        <v>700</v>
       </c>
     </row>
     <row r="57" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1874,7 +1914,7 @@
         <v>17</v>
       </c>
       <c r="F57" s="7">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="G57" s="7"/>
       <c r="H57" s="7">
@@ -1893,13 +1933,14 @@
         <v>16</v>
       </c>
       <c r="F58" s="7">
-        <v>1519.48</v>
-      </c>
-      <c r="G58" s="7">
-        <v>909.5</v>
+        <v>1321.53</v>
+      </c>
+      <c r="G58" s="12">
+        <f t="shared" ref="G58" si="8">(SUM(F57:F58)-SUM(H57:H58))</f>
+        <v>1521.5299999999997</v>
       </c>
       <c r="H58" s="7">
-        <v>600</v>
+        <v>700</v>
       </c>
     </row>
     <row r="59" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1914,7 +1955,7 @@
         <v>17</v>
       </c>
       <c r="F59" s="7">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="G59" s="7"/>
       <c r="H59" s="7">
@@ -1933,13 +1974,14 @@
         <v>16</v>
       </c>
       <c r="F60" s="7">
-        <v>1519.48</v>
-      </c>
-      <c r="G60" s="7">
-        <v>909.5</v>
+        <v>1321.53</v>
+      </c>
+      <c r="G60" s="12">
+        <f t="shared" ref="G60" si="9">(SUM(F59:F60)-SUM(H59:H60))</f>
+        <v>1521.5299999999997</v>
       </c>
       <c r="H60" s="7">
-        <v>600</v>
+        <v>700</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.3">
@@ -1950,16 +1992,16 @@
         <v>19</v>
       </c>
       <c r="F61" s="3">
-        <f>SUM(F3:F36)</f>
-        <v>48734.659999999996</v>
+        <f>SUM(F3:F50)</f>
+        <v>65713.179999999993</v>
       </c>
       <c r="G61" s="4">
         <f>G62/F61</f>
-        <v>0.66361127788723673</v>
+        <v>0.64400155341744225</v>
       </c>
       <c r="H61" s="4">
         <f>H62/F61</f>
-        <v>0.33261748414783238</v>
+        <v>0.35320159517466665</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.3">
@@ -1971,15 +2013,15 @@
       </c>
       <c r="F62" s="6">
         <f>SUM(F3:F60)</f>
-        <v>72968.420000000013</v>
+        <v>78320.829999999987</v>
       </c>
       <c r="G62" s="6">
-        <f>SUM(G3:G36)</f>
-        <v>32340.87</v>
+        <f>SUM(G3:G50)</f>
+        <v>42319.389999999992</v>
       </c>
       <c r="H62" s="6">
-        <f>SUM(H4:H36)</f>
-        <v>16210</v>
+        <f>SUM(H4:H50)</f>
+        <v>23210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>